<commit_message>
EXCEPTION 1 - 02 APRIL 2019: REMOVED 'PLAN DE DESCANSO'
</commit_message>
<xml_diff>
--- a/catalogoPlaza.xlsx
+++ b/catalogoPlaza.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="33" documentId="6_{08E79F67-B69A-4A8F-8577-019900AC34FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D17FBA58-4ACE-44F7-A7FF-4B22E14C07F1}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="-110" windowWidth="18380" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="-110" windowWidth="18380" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Offsite" sheetId="1" r:id="rId1"/>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8CF707-A19A-42B7-820C-9B9CDEB2C050}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAE905A-AC7F-4205-8AF5-5F8F0553EDF1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>